<commit_message>
feat: Docs nearly done
</commit_message>
<xml_diff>
--- a/docs/Evolution/ALLC ALLD TFT GRIM PAVLOV CONTRITE PROBER.xlsx
+++ b/docs/Evolution/ALLC ALLD TFT GRIM PAVLOV CONTRITE PROBER.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c1007595\Documents\Cpp\Miitto\IteratedPrisonersDilema\docs\Evolution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A4ED929A-DDB2-4DCF-8117-3F6DA0A066D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D467BA-BB04-4C9E-9BD8-E3B03F06ADBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{75CB45BB-0672-431A-BF54-0362F609B9D8}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="18105" activeTab="4" xr2:uid="{75CB45BB-0672-431A-BF54-0362F609B9D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Charts" sheetId="2" r:id="rId1"/>
     <sheet name="NoNoise" sheetId="3" r:id="rId2"/>
     <sheet name="0.05" sheetId="1" r:id="rId3"/>
+    <sheet name="SCB NoNoise" sheetId="4" r:id="rId4"/>
+    <sheet name="SCB 0.05" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="7">
   <si>
     <t>ALLC</t>
   </si>
@@ -607,7 +609,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -639,7 +641,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -686,6 +688,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'0.05'!$A$2:$A$51</c:f>
@@ -875,6 +931,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'0.05'!$B$2:$B$51</c:f>
@@ -1064,6 +1174,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'0.05'!$C$2:$C$51</c:f>
@@ -1253,6 +1417,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'0.05'!$D$2:$D$51</c:f>
@@ -1442,6 +1660,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'0.05'!$E$2:$E$51</c:f>
@@ -1631,6 +1903,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'0.05'!$F$2:$F$51</c:f>
@@ -1822,6 +2148,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>'0.05'!$G$2:$G$51</c:f>
@@ -1988,14 +2368,15 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="0"/>
         <c:overlap val="100"/>
         <c:axId val="407253328"/>
         <c:axId val="407254768"/>
@@ -2007,6 +2388,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2028,7 +2423,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2055,53 +2450,12 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="407253328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -2115,7 +2469,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2158,7 +2512,7 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -2210,7 +2564,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2224,11 +2578,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>No</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Noise</a:t>
+              <a:t>No Noise</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2246,7 +2596,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2293,6 +2643,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>NoNoise!$A$2:$A$51</c:f>
@@ -2482,6 +2886,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>NoNoise!$B$2:$B$51</c:f>
@@ -2671,6 +3129,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>NoNoise!$C$2:$C$51</c:f>
@@ -2860,6 +3372,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>NoNoise!$D$2:$D$51</c:f>
@@ -3049,6 +3615,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>NoNoise!$E$2:$E$51</c:f>
@@ -3238,6 +3858,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>NoNoise!$F$2:$F$51</c:f>
@@ -3429,6 +4103,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>NoNoise!$G$2:$G$51</c:f>
@@ -3595,14 +4323,15 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="0"/>
         <c:overlap val="100"/>
         <c:axId val="407657808"/>
         <c:axId val="407657328"/>
@@ -3614,6 +4343,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3635,7 +4378,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3662,53 +4405,12 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="407657808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -3722,7 +4424,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3765,7 +4467,7 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -3877,7 +4579,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="298">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3888,7 +4590,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -3911,18 +4613,18 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -3934,19 +4636,16 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -3978,35 +4677,45 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -4018,30 +4727,34 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -4063,15 +4776,13 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4081,7 +4792,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -4090,14 +4801,13 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -4106,17 +4816,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -4125,10 +4834,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
@@ -4144,21 +4853,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -4177,17 +4880,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -4196,17 +4898,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="50000"/>
             <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -4215,17 +4916,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -4246,7 +4946,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -4254,7 +4954,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -4267,6 +4967,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -4274,10 +4985,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -4298,7 +5009,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -4307,14 +5018,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -4328,27 +5039,26 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -4362,6 +5072,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -4369,20 +5090,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="298">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4393,7 +5108,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -4416,18 +5131,18 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -4439,19 +5154,16 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -4483,35 +5195,45 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -4523,30 +5245,34 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -4568,15 +5294,13 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4586,7 +5310,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -4595,14 +5319,13 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -4611,17 +5334,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -4630,10 +5352,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
@@ -4649,21 +5371,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -4682,17 +5398,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -4701,17 +5416,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="50000"/>
             <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -4720,17 +5434,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -4751,7 +5464,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -4759,7 +5472,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -4772,6 +5485,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -4779,10 +5503,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -4803,7 +5527,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -4812,14 +5536,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -4833,27 +5557,26 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -4867,6 +5590,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -4874,14 +5608,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -5286,8 +6014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B1662E-79D7-4CB1-8ACF-CAC343EC4F7F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7671,4 +8399,817 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D865123-9892-4377-9786-7ED439A7DA93}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>14</v>
+      </c>
+      <c r="F2">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>18</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>44</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>58</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>13</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>70</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>83</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>90</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>95</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>97</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDBBB115-47F9-45DA-83E6-5493F27ED5B7}">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>14</v>
+      </c>
+      <c r="F2">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>52</v>
+      </c>
+      <c r="B5">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>62</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>71</v>
+      </c>
+      <c r="B7">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>79</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>84</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>88</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>91</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>93</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>89</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>81</v>
+      </c>
+      <c r="B14">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>70</v>
+      </c>
+      <c r="B15">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>55</v>
+      </c>
+      <c r="B16">
+        <v>45</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>40</v>
+      </c>
+      <c r="B17">
+        <v>60</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>74</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>84</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="B20">
+        <v>91</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>95</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>97</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>99</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>99</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>